<commit_message>
Excel Data for USer and SkillMAP
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/UserAPIDataExcel.xlsx
+++ b/src/test/resources/ExcelData/UserAPIDataExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Baisali\eclipse-workspace\LMS_API_RestAssured\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Smita\NumpyNinja\HACKTHON-API\GitCode\LMS_API_RestAssured\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F53084-F641-4B23-8A9E-BE1EE821E695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96253A2C-4AD9-4CC3-B549-5D7330B9BB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="get" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="113">
   <si>
     <t>Value</t>
   </si>
@@ -63,9 +63,6 @@
     <t>null</t>
   </si>
   <si>
-    <t>U11</t>
-  </si>
-  <si>
     <t>u11</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Post data</t>
   </si>
   <si>
-    <t>U70</t>
-  </si>
-  <si>
     <t>67Sunnil,Kumar</t>
   </si>
   <si>
@@ -174,9 +168,6 @@
     <t>Alphanumeric location update data</t>
   </si>
   <si>
-    <t>Nisha,Singh</t>
-  </si>
-  <si>
     <t>Sneha,Patel</t>
   </si>
   <si>
@@ -282,18 +273,9 @@
     <t>Post data with invalid phone number</t>
   </si>
   <si>
-    <t>Baisali,Sadhukan</t>
-  </si>
-  <si>
-    <t>Portland</t>
-  </si>
-  <si>
     <t>Post Data</t>
   </si>
   <si>
-    <t>Janki78,Iyengar</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/Janki/</t>
   </si>
   <si>
@@ -352,13 +334,46 @@
   </si>
   <si>
     <t>validuserdata</t>
+  </si>
+  <si>
+    <t>alphanumericName</t>
+  </si>
+  <si>
+    <t>invalidPhone</t>
+  </si>
+  <si>
+    <t>invalidVisa</t>
+  </si>
+  <si>
+    <t>alphanumericLocation</t>
+  </si>
+  <si>
+    <t>Maggie Paul</t>
+  </si>
+  <si>
+    <t>Sandra Mark</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>H!</t>
+  </si>
+  <si>
+    <t>Priya23 prakash</t>
+  </si>
+  <si>
+    <t>U05</t>
+  </si>
+  <si>
+    <t>U07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -381,6 +396,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -657,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -671,13 +690,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -757,7 +776,7 @@
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -1767,7 +1786,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913DB920-4D59-4B57-AB12-C53654EB4241}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1784,69 +1805,69 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="K1" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="C2" s="3">
-        <v>2345672341</v>
+        <v>2345822341</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="K2">
         <v>201</v>
@@ -1854,32 +1875,32 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" s="3">
         <v>9776785678</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="I3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="K3">
         <v>400</v>
@@ -1887,34 +1908,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3">
         <v>9891285676</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K4">
         <v>400</v>
@@ -1922,34 +1943,34 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3">
         <v>4549985678</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="K5">
         <v>400</v>
@@ -1957,34 +1978,34 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3">
         <v>8646795600</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K6">
         <v>400</v>
@@ -1992,34 +2013,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3">
         <v>8846795678</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="K7">
         <v>400</v>
@@ -2027,34 +2048,34 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" s="3">
         <v>3217639090</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="K8">
         <v>400</v>
@@ -2062,34 +2083,34 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="K9">
         <v>400</v>
@@ -2097,32 +2118,32 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="C10" s="3">
-        <v>7899199375</v>
+        <v>7899149375</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K10">
         <v>201</v>
@@ -2130,32 +2151,32 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="C11" s="3">
-        <v>6007239924</v>
+        <v>6007233924</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="K11">
         <v>400</v>
@@ -2163,25 +2184,25 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C12" s="3">
         <v>9490615321</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12">
@@ -2190,7 +2211,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="K13">
         <v>400</v>
@@ -2214,9 +2235,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC952FE-9254-46D6-8BD2-8CB3D38E3D1D}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2227,202 +2250,236 @@
     <col min="10" max="10" width="28.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C2" s="3">
         <v>9089672321</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="C3" s="3">
+        <v>9089672321</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L3">
+        <v>400</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="3">
-        <v>7027864699</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="J4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>33</v>
+        <v>111</v>
+      </c>
+      <c r="L4">
+        <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3">
         <v>9089672321</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="J5" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>33</v>
+        <v>111</v>
+      </c>
+      <c r="L5">
+        <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3">
         <v>9089672321</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="K6" s="3" t="s">
-        <v>33</v>
+        <v>111</v>
+      </c>
+      <c r="L6">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{866C9FC6-5A6D-404E-9D85-4EBC6C3F8546}"/>
     <hyperlink ref="F4" r:id="rId2" xr:uid="{6DAE8628-761C-4C08-8E32-778223885C8E}"/>
@@ -2439,7 +2496,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2452,13 +2509,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2466,7 +2523,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="C2" s="7">
         <v>200</v>
@@ -2477,7 +2534,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="7">
         <v>404</v>
@@ -2494,10 +2551,10 @@
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="C5" s="7">
         <v>404</v>

</xml_diff>